<commit_message>
updated GC gas analysis
</commit_message>
<xml_diff>
--- a/data/bad_gc_list.xlsx
+++ b/data/bad_gc_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tacaro/Documents/GitHub/permafrost_LHSIP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968DB1C1-7784-FB40-AB69-A7307F7BA5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13217C38-1E01-CB42-9931-A4ECA4E0DF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{705A7CDB-22B9-F14D-ABBA-2A662AC6DD85}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{705A7CDB-22B9-F14D-ABBA-2A662AC6DD85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>file_name</t>
   </si>
@@ -153,9 +153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +193,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -299,7 +299,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -441,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2504AED3-A0D0-DA41-A856-FAEF54D31DB6}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="191" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,6 +555,11 @@
         <v>17</v>
       </c>
     </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>